<commit_message>
-Updated Excels for Experimento3
</commit_message>
<xml_diff>
--- a/Results/Experimento3[04_15_2023-15_01].xlsx
+++ b/Results/Experimento3[04_15_2023-15_01].xlsx
@@ -1,37 +1,126 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\Seminario\Codes\Datasets\MNIST_ORG\NN_Tests_DG\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C06D875-4534-46C5-BEAE-8F1A616528D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>val_acc_list</t>
+  </si>
+  <si>
+    <t>test_acc</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>lr</t>
+  </si>
+  <si>
+    <t>val_acc</t>
+  </si>
+  <si>
+    <t>[0, 0.387, 0.4252, 0.6408, 0.689, 0.5974, 0.791, 0.7842, 0.8246, 0.8266, 0.7642, 0.7378, 0.788, 0.7558, 0.7982, 0.8402, 0.8464, 0.86, 0.7648, 0.7544, 0.8068, 0.813, 0.8222, 0.8636, 0.869, 0.8786, 0.8386, 0.7578, 0.8226, 0.8258, 0.8026, 0.845, 0.8832, 0.884, 0.8756, 0.8448, 0.8058, 0.8384, 0.881, 0.8808, 0.8822, 0.8842, 0.8742, 0.8334, 0.8274, 0.8282, 0.8734, 0.8766, 0.8784, 0.8814, 0.8656]</t>
+  </si>
+  <si>
+    <t>86.12%</t>
+  </si>
+  <si>
+    <t>[1.8485413312911987, 2.0524969935417174, 0.9892231345176696, 0.9233922481536865, 1.3946666836738586, 0.6190386116504669, 0.6400498867034912, 0.5224890559911728, 0.5130460739135743, 0.717246800661087, 0.806268161535263, 0.662273770570755, 0.7589650452136993, 0.5983486533164978, 0.47592452466487883, 0.4692301839590073, 0.4362915366888046, 0.7650841414928437, 0.8461125373840332, 0.6390454471111298, 0.6078792214393616, 0.5915754675865174, 0.4556849956512451, 0.44179199934005736, 0.42907099723815917, 0.5416705131530761, 0.8207585573196411, 0.5843209445476532, 0.5514320582151413, 0.7097763001918793, 0.5115257054567337, 0.4115972429513931, 0.4231680452823639, 0.4473858118057251, 0.5666245132684707, 0.7075292468070984, 0.5892319470643997, 0.4262721389532089, 0.4405135214328766, 0.44444176852703093, 0.4468920320272446, 0.49353104531764985, 0.5971766918897629, 0.6242875397205353, 0.637197071313858, 0.4629494071006775, 0.46921705901622773, 0.47244237661361693, 0.45953304767608644, 0.5309466600418091]</t>
+  </si>
+  <si>
+    <t>[0.03838321292402648, 0.054439595543727806, 0.05782287328110407, 0.0835784565271562, 0.03178907489885383, 0.030992133383586085, 0.012555729571778319, 0.009651402002653435, 0.05006272498869055, 0.0626236465497018, 0.0844296348983031, 0.09880602607633178, 0.06339062042459054, 0.029294026875732286, 0.028529055182063334, 0.013022849094944772, 0.0544026698048812, 0.07864577558653586, 0.07992212302895806, 0.08446264074753655, 0.046923317117484785, 0.029462182962133113, 0.01660191625806228, 0.010951465873999833, 0.051289804783998964, 0.08252471318164026, 0.09755735368658576, 0.09875403616265106, 0.09166372230046281, 0.0729796643240951, 0.023387664042790933, 0.019453016924752754, 0.029951449482181265, 0.06924015601889, 0.0966477388021667, 0.09688296286387003, 0.018695511705244562, 0.0169782333929489, 0.012675435083854204, 0.011450765139857603, 0.03208945726761333, 0.09566230504270393, 0.09964825969799268, 0.10091354557821511, 0.03862960171632205, 0.029168704967379618, 0.029152055391656703, 0.0156658151119021, 0.06125073444961583, 0.08765865926549793]</t>
+  </si>
+  <si>
+    <t>86.56%</t>
+  </si>
+  <si>
+    <t>[0, 0.1852, 0.3556, 0.4444, 0.5622, 0.5838, 0.6254, 0.7076, 0.7314, 0.7238, 0.781, 0.7988, 0.8008, 0.7936, 0.7966, 0.8072, 0.8058, 0.8296, 0.8058, 0.8354, 0.8302, 0.837, 0.837, 0.8316, 0.8488, 0.847, 0.8414, 0.8444, 0.8484, 0.8408, 0.8538, 0.8502, 0.8454, 0.8574, 0.8414, 0.8436, 0.8556, 0.8372, 0.821, 0.8374, 0.8476, 0.8516, 0.8558, 0.8536, 0.8318, 0.8686, 0.847, 0.85, 0.8416, 0.86, 0.857]</t>
+  </si>
+  <si>
+    <t>85.96%</t>
+  </si>
+  <si>
+    <t>[2.1786319971084596, 1.7001827120780946, 1.498991858959198, 1.2349929451942443, 1.2335974335670472, 1.0568583309650421, 0.8354133784770965, 0.7843111395835877, 0.8309636235237121, 0.6463446974754333, 0.6202138602733612, 0.5898355782032013, 0.5965407013893127, 0.6212744832038879, 0.58788583278656, 0.6109933078289032, 0.5156726002693176, 0.6437571942806244, 0.5160220682621002, 0.5429224729537964, 0.5245403975248337, 0.5462483793497086, 0.5152780741453171, 0.4924091637134552, 0.48103746175765993, 0.5426326125860215, 0.5454978555440902, 0.5273589432239533, 0.5353526115417481, 0.4730619341135025, 0.5057766228914261, 0.5188775777816772, 0.480952051281929, 0.5893720656633377, 0.5516750156879425, 0.5242258757352829, 0.6250744342803956, 0.7068353235721588, 0.643314751982689, 0.6052718043327332, 0.5645631790161133, 0.5438005864620209, 0.5736543595790863, 0.6269943237304687, 0.5056281864643097, 0.5588747739791871, 0.5969744622707367, 0.6695210933685303, 0.5419950723648072, 0.5894211411476136]</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>[0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01]</t>
+  </si>
+  <si>
+    <t>85.7%</t>
+  </si>
+  <si>
+    <t>[0, 0.343, 0.4654, 0.537, 0.6214, 0.6394, 0.7248, 0.751, 0.757, 0.7962, 0.7964, 0.8038, 0.8092, 0.8106, 0.8084, 0.8156, 0.8048, 0.813, 0.815, 0.82, 0.8104, 0.8194, 0.8078, 0.8126, 0.8096, 0.8148, 0.8084, 0.8186, 0.8196, 0.8242, 0.8154, 0.8208, 0.8056, 0.822, 0.8186, 0.83, 0.8046, 0.8266, 0.8052, 0.823, 0.8082, 0.8236, 0.8104, 0.828, 0.8104, 0.8228, 0.8118, 0.8206, 0.8134, 0.8224, 0.8236]</t>
+  </si>
+  <si>
+    <t>82.06%</t>
+  </si>
+  <si>
+    <t>[1.7236761927604676, 1.441059410572052, 1.2637874245643617, 1.0662525713443756, 1.0169091820716858, 0.7807262778282166, 0.7228374063968659, 0.6840186953544617, 0.5969401061534881, 0.5936563968658447, 0.5643043667078018, 0.571885484457016, 0.5574630111455917, 0.5659029126167298, 0.5442533731460572, 0.5693890869617462, 0.5453902810811997, 0.5607354491949081, 0.5399384886026383, 0.5793227255344391, 0.5422226846218109, 0.6011863946914673, 0.5487987369298934, 0.565973311662674, 0.5328830868005753, 0.5889648556709289, 0.5393567085266113, 0.5607105940580368, 0.5464304536581039, 0.5567595005035401, 0.5388839334249497, 0.6162800788879395, 0.5498103588819504, 0.5685970216989518, 0.5369456559419632, 0.6519876837730407, 0.5531337112188339, 0.6295345664024353, 0.5524795651435852, 0.6308235049247741, 0.5566228091716766, 0.6277609467506409, 0.5585093110799789, 0.6179499745368957, 0.5636664450168609, 0.6265789866447449, 0.5821062326431274, 0.597978127002716, 0.5642197102308273, 0.5812352687120438]</t>
+  </si>
+  <si>
+    <t>[0.09000000000000001, 0.08000000000000002, 0.07000000000000002, 0.06000000000000002, 0.05000000000000002, 0.040000000000000015, 0.030000000000000013, 0.02000000000000001, 0.01000000000000001, 1.0408340855860843e-17, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0]</t>
+  </si>
+  <si>
+    <t>82.36%</t>
+  </si>
+  <si>
+    <t>TA Ciclica Aleatoria Ext</t>
+  </si>
+  <si>
+    <t>TA Decreciente (propuesta)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +135,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,173 +459,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="45.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>val_acc_list</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>test_acc</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>cost</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>epochs</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>lr</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>val_acc</t>
-        </is>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>[0, 0.387, 0.4252, 0.6408, 0.689, 0.5974, 0.791, 0.7842, 0.8246, 0.8266, 0.7642, 0.7378, 0.788, 0.7558, 0.7982, 0.8402, 0.8464, 0.86, 0.7648, 0.7544, 0.8068, 0.813, 0.8222, 0.8636, 0.869, 0.8786, 0.8386, 0.7578, 0.8226, 0.8258, 0.8026, 0.845, 0.8832, 0.884, 0.8756, 0.8448, 0.8058, 0.8384, 0.881, 0.8808, 0.8822, 0.8842, 0.8742, 0.8334, 0.8274, 0.8282, 0.8734, 0.8766, 0.8784, 0.8814, 0.8656]</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>86.12%</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>[1.8485413312911987, 2.0524969935417174, 0.9892231345176696, 0.9233922481536865, 1.3946666836738586, 0.6190386116504669, 0.6400498867034912, 0.5224890559911728, 0.5130460739135743, 0.717246800661087, 0.806268161535263, 0.662273770570755, 0.7589650452136993, 0.5983486533164978, 0.47592452466487883, 0.4692301839590073, 0.4362915366888046, 0.7650841414928437, 0.8461125373840332, 0.6390454471111298, 0.6078792214393616, 0.5915754675865174, 0.4556849956512451, 0.44179199934005736, 0.42907099723815917, 0.5416705131530761, 0.8207585573196411, 0.5843209445476532, 0.5514320582151413, 0.7097763001918793, 0.5115257054567337, 0.4115972429513931, 0.4231680452823639, 0.4473858118057251, 0.5666245132684707, 0.7075292468070984, 0.5892319470643997, 0.4262721389532089, 0.4405135214328766, 0.44444176852703093, 0.4468920320272446, 0.49353104531764985, 0.5971766918897629, 0.6242875397205353, 0.637197071313858, 0.4629494071006775, 0.46921705901622773, 0.47244237661361693, 0.45953304767608644, 0.5309466600418091]</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
         <v>2671160.25</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Random Ciclico Extended</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>[0.03838321292402648, 0.054439595543727806, 0.05782287328110407, 0.0835784565271562, 0.03178907489885383, 0.030992133383586085, 0.012555729571778319, 0.009651402002653435, 0.05006272498869055, 0.0626236465497018, 0.0844296348983031, 0.09880602607633178, 0.06339062042459054, 0.029294026875732286, 0.028529055182063334, 0.013022849094944772, 0.0544026698048812, 0.07864577558653586, 0.07992212302895806, 0.08446264074753655, 0.046923317117484785, 0.029462182962133113, 0.01660191625806228, 0.010951465873999833, 0.051289804783998964, 0.08252471318164026, 0.09755735368658576, 0.09875403616265106, 0.09166372230046281, 0.0729796643240951, 0.023387664042790933, 0.019453016924752754, 0.029951449482181265, 0.06924015601889, 0.0966477388021667, 0.09688296286387003, 0.018695511705244562, 0.0169782333929489, 0.012675435083854204, 0.011450765139857603, 0.03208945726761333, 0.09566230504270393, 0.09964825969799268, 0.10091354557821511, 0.03862960171632205, 0.029168704967379618, 0.029152055391656703, 0.0156658151119021, 0.06125073444961583, 0.08765865926549793]</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>86.56%</t>
-        </is>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>[0, 0.1852, 0.3556, 0.4444, 0.5622, 0.5838, 0.6254, 0.7076, 0.7314, 0.7238, 0.781, 0.7988, 0.8008, 0.7936, 0.7966, 0.8072, 0.8058, 0.8296, 0.8058, 0.8354, 0.8302, 0.837, 0.837, 0.8316, 0.8488, 0.847, 0.8414, 0.8444, 0.8484, 0.8408, 0.8538, 0.8502, 0.8454, 0.8574, 0.8414, 0.8436, 0.8556, 0.8372, 0.821, 0.8374, 0.8476, 0.8516, 0.8558, 0.8536, 0.8318, 0.8686, 0.847, 0.85, 0.8416, 0.86, 0.857]</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>85.96%</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>[2.1786319971084596, 1.7001827120780946, 1.498991858959198, 1.2349929451942443, 1.2335974335670472, 1.0568583309650421, 0.8354133784770965, 0.7843111395835877, 0.8309636235237121, 0.6463446974754333, 0.6202138602733612, 0.5898355782032013, 0.5965407013893127, 0.6212744832038879, 0.58788583278656, 0.6109933078289032, 0.5156726002693176, 0.6437571942806244, 0.5160220682621002, 0.5429224729537964, 0.5245403975248337, 0.5462483793497086, 0.5152780741453171, 0.4924091637134552, 0.48103746175765993, 0.5426326125860215, 0.5454978555440902, 0.5273589432239533, 0.5353526115417481, 0.4730619341135025, 0.5057766228914261, 0.5188775777816772, 0.480952051281929, 0.5893720656633377, 0.5516750156879425, 0.5242258757352829, 0.6250744342803956, 0.7068353235721588, 0.643314751982689, 0.6052718043327332, 0.5645631790161133, 0.5438005864620209, 0.5736543595790863, 0.6269943237304687, 0.5056281864643097, 0.5588747739791871, 0.5969744622707367, 0.6695210933685303, 0.5419950723648072, 0.5894211411476136]</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
         <v>2733489.5</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Adam</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>[0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01, 0.01]</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>85.7%</t>
-        </is>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>[0, 0.343, 0.4654, 0.537, 0.6214, 0.6394, 0.7248, 0.751, 0.757, 0.7962, 0.7964, 0.8038, 0.8092, 0.8106, 0.8084, 0.8156, 0.8048, 0.813, 0.815, 0.82, 0.8104, 0.8194, 0.8078, 0.8126, 0.8096, 0.8148, 0.8084, 0.8186, 0.8196, 0.8242, 0.8154, 0.8208, 0.8056, 0.822, 0.8186, 0.83, 0.8046, 0.8266, 0.8052, 0.823, 0.8082, 0.8236, 0.8104, 0.828, 0.8104, 0.8228, 0.8118, 0.8206, 0.8134, 0.8224, 0.8236]</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>82.06%</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>[1.7236761927604676, 1.441059410572052, 1.2637874245643617, 1.0662525713443756, 1.0169091820716858, 0.7807262778282166, 0.7228374063968659, 0.6840186953544617, 0.5969401061534881, 0.5936563968658447, 0.5643043667078018, 0.571885484457016, 0.5574630111455917, 0.5659029126167298, 0.5442533731460572, 0.5693890869617462, 0.5453902810811997, 0.5607354491949081, 0.5399384886026383, 0.5793227255344391, 0.5422226846218109, 0.6011863946914673, 0.5487987369298934, 0.565973311662674, 0.5328830868005753, 0.5889648556709289, 0.5393567085266113, 0.5607105940580368, 0.5464304536581039, 0.5567595005035401, 0.5388839334249497, 0.6162800788879395, 0.5498103588819504, 0.5685970216989518, 0.5369456559419632, 0.6519876837730407, 0.5531337112188339, 0.6295345664024353, 0.5524795651435852, 0.6308235049247741, 0.5566228091716766, 0.6277609467506409, 0.5585093110799789, 0.6179499745368957, 0.5636664450168609, 0.6265789866447449, 0.5821062326431274, 0.597978127002716, 0.5642197102308273, 0.5812352687120438]</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
         <v>2669289.25</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Nuestro decreciente con Momentum</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>[0.09000000000000001, 0.08000000000000002, 0.07000000000000002, 0.06000000000000002, 0.05000000000000002, 0.040000000000000015, 0.030000000000000013, 0.02000000000000001, 0.01000000000000001, 1.0408340855860843e-17, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0, 0.01, 0.0]</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>82.36%</t>
-        </is>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>